<commit_message>
copy class from another done
</commit_message>
<xml_diff>
--- a/Nová položka Hárok Microsoft Excelu.xlsx
+++ b/Nová položka Hárok Microsoft Excelu.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6787D7CB-089B-48C7-92AA-D24EFA5569D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8504D010-9081-405B-AA5D-C76F853D51E6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
   <si>
     <t>Feature</t>
   </si>
@@ -212,6 +212,21 @@
   </si>
   <si>
     <t>Práca s kliknutiami a klavesami</t>
+  </si>
+  <si>
+    <t>DragNDropClass</t>
+  </si>
+  <si>
+    <t>Copy Class</t>
+  </si>
+  <si>
+    <t>skopiruje classu z jednej tabule do druhej</t>
+  </si>
+  <si>
+    <t>hold ,,F" + click na classu , potom hold ,,F" click na tabulu</t>
+  </si>
+  <si>
+    <t>*neni su osetrene corner cases</t>
   </si>
 </sst>
 </file>
@@ -281,12 +296,12 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -570,273 +585,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="42.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="53.109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="53.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>